<commit_message>
Added Fallback, Resilience and Distributed Tracing etc.
</commit_message>
<xml_diff>
--- a/Project_MicroServices.xlsx
+++ b/Project_MicroServices.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Java_Code\Bank_RabbitMQ_Docker_K8_Helm_Istio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786A6544-AB21-4B42-902F-B0D7C0244086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8BD6A4-DAC7-4AFA-B6E5-9728E9FC0E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="726" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Application-Ports" sheetId="1" r:id="rId1"/>
     <sheet name="Refresh_Config_Runtime" sheetId="2" r:id="rId2"/>
     <sheet name="Spring-Cloud" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
-    <sheet name="API-Gateway" sheetId="6" r:id="rId5"/>
-    <sheet name="Eureka" sheetId="5" r:id="rId6"/>
+    <sheet name="Retry" sheetId="8" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId5"/>
+    <sheet name="Monitor_Observe" sheetId="9" r:id="rId6"/>
+    <sheet name="API-Gateway" sheetId="6" r:id="rId7"/>
+    <sheet name="Patterns" sheetId="7" r:id="rId8"/>
+    <sheet name="Eureka" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
   <si>
     <t>Accounts</t>
   </si>
@@ -274,6 +277,134 @@
   </si>
   <si>
     <t>SpringCloudAPIGateway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API Gateway </t>
+  </si>
+  <si>
+    <t>Gateway Routing Pattern</t>
+  </si>
+  <si>
+    <t>route incoming client requests to backend services based on URL, Headers or Request Parameters.</t>
+  </si>
+  <si>
+    <t>Gateway Offloading Pattern</t>
+  </si>
+  <si>
+    <t>Backend for Front End</t>
+  </si>
+  <si>
+    <t>separate Backend service is created for different Front end.</t>
+  </si>
+  <si>
+    <t>API Gateway consolidates requests into a single Response.</t>
+  </si>
+  <si>
+    <t>Design Patterns</t>
+  </si>
+  <si>
+    <t>define a strategy to delay retries to avoid overwhelming the system.</t>
+  </si>
+  <si>
+    <t>Retry Logic</t>
+  </si>
+  <si>
+    <t>a) Backoff Strategy</t>
+  </si>
+  <si>
+    <t>b) Circuit Breaker Integration</t>
+  </si>
+  <si>
+    <t>c) Idempotent Operations</t>
+  </si>
+  <si>
+    <t>Ensure retried operation is idempotent.</t>
+  </si>
+  <si>
+    <t>If certain # of retries fail, open the circuit to prevent further requests.</t>
+  </si>
+  <si>
+    <t>When and how many times to retry an operation.</t>
+  </si>
+  <si>
+    <t>Redis Rate limiter pattern</t>
+  </si>
+  <si>
+    <t>Bulkhead</t>
+  </si>
+  <si>
+    <t>Gateway Aggregator / Composition Pattern</t>
+  </si>
+  <si>
+    <t>isolate and limit impact of failures/high loads in 1 component from spreading to other components. It is useful in Systems that require high availability, fault tolerance and isolation between components.</t>
+  </si>
+  <si>
+    <t>Observability</t>
+  </si>
+  <si>
+    <t>Record of events that occur in a System. 
+Track errors, exceptions and unexpected events.</t>
+  </si>
+  <si>
+    <t>Health of System - CPU usage, memory and response times.</t>
+  </si>
+  <si>
+    <t>Path that a request takes through the System.</t>
+  </si>
+  <si>
+    <t>Monitoring</t>
+  </si>
+  <si>
+    <t>Identify / Troubleshoot Problems</t>
+  </si>
+  <si>
+    <t>Collect and analyze data from Microservices.</t>
+  </si>
+  <si>
+    <t>Track health of Microservices</t>
+  </si>
+  <si>
+    <t>Optimize Microservices</t>
+  </si>
+  <si>
+    <t>Optimize Microservices to improve performance and reliability.</t>
+  </si>
+  <si>
+    <t>Identify Microservices that are underperforming or having problems.</t>
+  </si>
+  <si>
+    <t>Metrics - pillar 1</t>
+  </si>
+  <si>
+    <t>Logs - pillar 2</t>
+  </si>
+  <si>
+    <t>Traces - pillar 3</t>
+  </si>
+  <si>
+    <t>Logs from many Microservices are stored in central location.</t>
+  </si>
+  <si>
+    <t>Grafana</t>
+  </si>
+  <si>
+    <t>open source analytics and 
+interactive visual web application.</t>
+  </si>
+  <si>
+    <t>It provides Charts, Graphs an Alerts for Web when connected to supported data sources.</t>
+  </si>
+  <si>
+    <t>lightweight log agent that ships logs from your containers to Loki. It is easy to configure and collect logs from a variety of sources.</t>
+  </si>
+  <si>
+    <t>Grafana Loki - DB</t>
+  </si>
+  <si>
+    <t>horizontally scalable, highly available and cost effective log aggregation system or Database.</t>
+  </si>
+  <si>
+    <t>Promtail (replaced by Alloy)</t>
   </si>
 </sst>
 </file>
@@ -327,7 +458,7 @@
       <name val="JetBrains Mono"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,8 +477,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -370,11 +507,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -400,6 +548,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,85 +849,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:D10"/>
+  <dimension ref="C1:I11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:4">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="8:9">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="3:4">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="8:9">
+      <c r="H2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4">
+      <c r="I2" s="4">
         <v>8200</v>
       </c>
     </row>
-    <row r="3" spans="3:4">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="8:9">
+      <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="I3" s="4">
         <v>8201</v>
       </c>
     </row>
-    <row r="4" spans="3:4">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="8:9">
+      <c r="H4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4">
+      <c r="I4" s="4">
         <v>8202</v>
       </c>
     </row>
-    <row r="5" spans="3:4">
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="8:9">
+      <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4">
+      <c r="I5" s="4">
         <v>8071</v>
       </c>
     </row>
-    <row r="6" spans="3:4">
-      <c r="C6" s="1" t="s">
+    <row r="6" spans="8:9">
+      <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="I6" s="6">
         <v>8761</v>
       </c>
     </row>
-    <row r="7" spans="3:4">
-      <c r="C7" s="1" t="s">
+    <row r="7" spans="8:9">
+      <c r="H7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="4">
+      <c r="I7" s="4">
         <v>8203</v>
       </c>
     </row>
-    <row r="8" spans="3:4">
-      <c r="C8" s="1"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="3:4">
-      <c r="C9" s="1"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="3:4">
-      <c r="C10" s="1"/>
-      <c r="D10" s="4"/>
+    <row r="8" spans="8:9">
+      <c r="H8" s="1"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="8:9">
+      <c r="H9" s="1"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="8:9">
+      <c r="H10" s="1"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="8:9">
+      <c r="I11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -877,6 +1050,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E84C1293-D0A0-4394-AA51-32A21A6B91EE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4633BF0C-3C03-48DF-B774-96199D47C97F}">
   <dimension ref="E1:F8"/>
   <sheetViews>
@@ -943,7 +1128,133 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8D6997-4137-45D8-A6EA-F1F4C4F33E71}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="30">
+      <c r="A9" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B6842BD-085B-4657-AFCF-DA25B2750A24}">
   <dimension ref="I1:I10"/>
   <sheetViews>
@@ -1007,11 +1318,123 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B7B7B9-C4A0-4F74-9CD0-0026C29CE0C9}">
+  <dimension ref="E1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="93.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="5:6">
+      <c r="E1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="5:6">
+      <c r="E2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="5:6">
+      <c r="E3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="5:6">
+      <c r="E4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="5:6">
+      <c r="E5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="5:6">
+      <c r="E6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="5:6">
+      <c r="E7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="5:6" ht="32.25" customHeight="1">
+      <c r="E8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="5:6">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="5:6">
+      <c r="E10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="5:6">
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="5:6">
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="5:6">
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0417EE4-F03E-4BBD-8CB1-2F82B9F09EC1}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>